<commit_message>
Updated csv and xlsx files
</commit_message>
<xml_diff>
--- a/processed_data.xlsx
+++ b/processed_data.xlsx
@@ -472,10 +472,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>39332</v>
+        <v>38760</v>
       </c>
       <c r="D2" t="n">
-        <v>719426.73</v>
+        <v>709282.13</v>
       </c>
       <c r="E2" t="n">
         <v>60423</v>
@@ -491,10 +491,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>21417</v>
+        <v>21115</v>
       </c>
       <c r="D3" t="n">
-        <v>392974.17</v>
+        <v>387399.07</v>
       </c>
       <c r="E3" t="n">
         <v>33192</v>
@@ -510,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>47360</v>
+        <v>46591</v>
       </c>
       <c r="D4" t="n">
-        <v>863175.77</v>
+        <v>849272.37</v>
       </c>
       <c r="E4" t="n">
         <v>72356</v>
@@ -529,10 +529,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>22111</v>
+        <v>21762</v>
       </c>
       <c r="D5" t="n">
-        <v>402962.52</v>
+        <v>396681.62</v>
       </c>
       <c r="E5" t="n">
         <v>35025</v>
@@ -548,10 +548,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>78518</v>
+        <v>77375</v>
       </c>
       <c r="D6" t="n">
-        <v>1428712.23</v>
+        <v>1408245.68</v>
       </c>
       <c r="E6" t="n">
         <v>120148</v>
@@ -567,10 +567,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>31347</v>
+        <v>30871</v>
       </c>
       <c r="D7" t="n">
-        <v>573135.0699999999</v>
+        <v>564570.27</v>
       </c>
       <c r="E7" t="n">
         <v>48879</v>
@@ -632,10 +632,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1541386</v>
+        <v>1506926</v>
       </c>
       <c r="D2" t="n">
-        <v>3946184.47</v>
+        <v>3864197.5</v>
       </c>
       <c r="E2" t="n">
         <v>2092667</v>
@@ -651,10 +651,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>644115</v>
+        <v>630653</v>
       </c>
       <c r="D3" t="n">
-        <v>1789107.05</v>
+        <v>1753631.14</v>
       </c>
       <c r="E3" t="n">
         <v>944520</v>
@@ -670,13 +670,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1857723</v>
+        <v>1817418</v>
       </c>
       <c r="D4" t="n">
-        <v>4790122.99</v>
+        <v>4692244.73</v>
       </c>
       <c r="E4" t="n">
-        <v>2531664</v>
+        <v>2531662</v>
       </c>
     </row>
     <row r="5">
@@ -689,10 +689,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>779249</v>
+        <v>762316</v>
       </c>
       <c r="D5" t="n">
-        <v>2130791.24</v>
+        <v>2086748.89</v>
       </c>
       <c r="E5" t="n">
         <v>1139972</v>
@@ -708,13 +708,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2371166</v>
+        <v>2320330</v>
       </c>
       <c r="D6" t="n">
-        <v>6454670.34</v>
+        <v>6323928.79</v>
       </c>
       <c r="E6" t="n">
-        <v>3227982</v>
+        <v>3227981</v>
       </c>
     </row>
     <row r="7">
@@ -727,10 +727,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>810125</v>
+        <v>792865</v>
       </c>
       <c r="D7" t="n">
-        <v>2311240.52</v>
+        <v>2264608.14</v>
       </c>
       <c r="E7" t="n">
         <v>1185602</v>
@@ -792,10 +792,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>12119</v>
+        <v>12023</v>
       </c>
       <c r="D2" t="n">
-        <v>164787.09</v>
+        <v>163111.66</v>
       </c>
       <c r="E2" t="n">
         <v>15593</v>
@@ -811,10 +811,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>5319</v>
+        <v>5257</v>
       </c>
       <c r="D3" t="n">
-        <v>75398.67999999999</v>
+        <v>74651.24000000001</v>
       </c>
       <c r="E3" t="n">
         <v>7666</v>
@@ -830,10 +830,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>14506</v>
+        <v>14373</v>
       </c>
       <c r="D4" t="n">
-        <v>191410.52</v>
+        <v>189633.38</v>
       </c>
       <c r="E4" t="n">
         <v>18149</v>
@@ -849,10 +849,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>5482</v>
+        <v>5425</v>
       </c>
       <c r="D5" t="n">
-        <v>76067.82000000001</v>
+        <v>75294.38</v>
       </c>
       <c r="E5" t="n">
         <v>7602</v>
@@ -868,10 +868,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>20520</v>
+        <v>20288</v>
       </c>
       <c r="D6" t="n">
-        <v>289255.61</v>
+        <v>285533.96</v>
       </c>
       <c r="E6" t="n">
         <v>26537</v>
@@ -887,10 +887,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>6951</v>
+        <v>6868</v>
       </c>
       <c r="D7" t="n">
-        <v>102889.69</v>
+        <v>101585.84</v>
       </c>
       <c r="E7" t="n">
         <v>10118</v>

</xml_diff>

<commit_message>
Removed apply methods and refactor code
</commit_message>
<xml_diff>
--- a/processed_data.xlsx
+++ b/processed_data.xlsx
@@ -438,7 +438,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>year_month</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -472,13 +472,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>38760</v>
+        <v>40937</v>
       </c>
       <c r="D2" t="n">
-        <v>709282.13</v>
+        <v>749144.01</v>
       </c>
       <c r="E2" t="n">
-        <v>60423</v>
+        <v>63641</v>
       </c>
     </row>
     <row r="3">
@@ -510,13 +510,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>46591</v>
+        <v>49903</v>
       </c>
       <c r="D4" t="n">
-        <v>849272.37</v>
+        <v>909913.16</v>
       </c>
       <c r="E4" t="n">
-        <v>72356</v>
+        <v>77372</v>
       </c>
     </row>
     <row r="5">
@@ -548,13 +548,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>77375</v>
+        <v>77429</v>
       </c>
       <c r="D6" t="n">
-        <v>1408245.68</v>
+        <v>1409270.6</v>
       </c>
       <c r="E6" t="n">
-        <v>120148</v>
+        <v>120217</v>
       </c>
     </row>
     <row r="7">
@@ -598,7 +598,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>year_month</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -632,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1506926</v>
+        <v>1582901</v>
       </c>
       <c r="D2" t="n">
-        <v>3864197.5</v>
+        <v>4076706.02</v>
       </c>
       <c r="E2" t="n">
-        <v>2092667</v>
+        <v>2197129</v>
       </c>
     </row>
     <row r="3">
@@ -670,13 +670,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1817418</v>
+        <v>1908848</v>
       </c>
       <c r="D4" t="n">
-        <v>4692244.73</v>
+        <v>4950829.53</v>
       </c>
       <c r="E4" t="n">
-        <v>2531662</v>
+        <v>2658010</v>
       </c>
     </row>
     <row r="5">
@@ -708,13 +708,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2320330</v>
+        <v>2320784</v>
       </c>
       <c r="D6" t="n">
-        <v>6323928.79</v>
+        <v>6326754.48</v>
       </c>
       <c r="E6" t="n">
-        <v>3227981</v>
+        <v>3228655</v>
       </c>
     </row>
     <row r="7">
@@ -758,7 +758,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>year_month</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -792,13 +792,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>12023</v>
+        <v>12792</v>
       </c>
       <c r="D2" t="n">
-        <v>163111.66</v>
+        <v>173169.86</v>
       </c>
       <c r="E2" t="n">
-        <v>15593</v>
+        <v>16532</v>
       </c>
     </row>
     <row r="3">
@@ -830,13 +830,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>14373</v>
+        <v>15274</v>
       </c>
       <c r="D4" t="n">
-        <v>189633.38</v>
+        <v>202062.68</v>
       </c>
       <c r="E4" t="n">
-        <v>18149</v>
+        <v>19335</v>
       </c>
     </row>
     <row r="5">
@@ -868,13 +868,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>20288</v>
+        <v>20292</v>
       </c>
       <c r="D6" t="n">
-        <v>285533.96</v>
+        <v>285632.9</v>
       </c>
       <c r="E6" t="n">
-        <v>26537</v>
+        <v>26542</v>
       </c>
     </row>
     <row r="7">

</xml_diff>